<commit_message>
Ajout image assemblage + conversion
</commit_message>
<xml_diff>
--- a/CR - Cost Report/BOM/ST/STA0100,STA0400_to_STA0500.xlsx
+++ b/CR - Cost Report/BOM/ST/STA0100,STA0400_to_STA0500.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Optimus_2019\STUF2019\CR - Cost Report\BOM\ST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guillaume Touzé\Documents\GitHub\STUF2019\CR - Cost Report\BOM\ST\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B7D14F-0DC8-4AAF-8C7B-926F792B4E12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -87,12 +88,6 @@
     <t>ST</t>
   </si>
   <si>
-    <t>ST_A0001</t>
-  </si>
-  <si>
-    <t>ST_A0004</t>
-  </si>
-  <si>
     <t>ST_01001</t>
   </si>
   <si>
@@ -147,9 +142,6 @@
     <t>ST_04006</t>
   </si>
   <si>
-    <t>ST_A0005</t>
-  </si>
-  <si>
     <t>Steering wheel</t>
   </si>
   <si>
@@ -169,12 +161,21 @@
   </si>
   <si>
     <t>Tapped, glued to carbon tube</t>
+  </si>
+  <si>
+    <t>ST_A0100</t>
+  </si>
+  <si>
+    <t>ST_A0400</t>
+  </si>
+  <si>
+    <t>ST_A0500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -574,12 +575,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,31 +623,31 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -665,7 +666,7 @@
         <v>9</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -684,7 +685,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -703,7 +704,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -722,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -741,7 +742,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -749,14 +750,14 @@
         <v>11</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -775,7 +776,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -794,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -813,7 +814,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -832,7 +833,7 @@
         <v>9</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -851,7 +852,7 @@
         <v>9</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -870,7 +871,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -878,33 +879,33 @@
         <v>11</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -923,7 +924,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -942,7 +943,7 @@
         <v>9</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -961,7 +962,7 @@
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -980,7 +981,7 @@
         <v>9</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -999,7 +1000,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>